<commit_message>
add session cover page.
</commit_message>
<xml_diff>
--- a/input-aini2016.xlsx
+++ b/input-aini2016.xlsx
@@ -9,12 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10635" yWindow="3195" windowWidth="38520" windowHeight="22305" tabRatio="500"/>
+    <workbookView xWindow="2925" yWindow="9585" windowWidth="33045" windowHeight="17280" tabRatio="330"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AINI 2016 Abstract Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'AINI 2016 Abstract Data'!$D$1:$O$1</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'AINI 2016 Abstract Data'!$D$1:$O$1</definedName>
+  </definedNames>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,22 +29,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>Program No.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Program No. Long</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Affiliation</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Figure file Name</t>
+    <phoneticPr fontId="6"/>
+  </si>
   <si>
     <t>Title</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="6"/>
   </si>
   <si>
     <t>Name</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="6"/>
   </si>
   <si>
     <t>e-mail</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="6"/>
   </si>
   <si>
     <t>DOI</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Registration No.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>References</t>
+    <phoneticPr fontId="6"/>
   </si>
   <si>
     <t>Abstract</t>
@@ -47,38 +76,18 @@
   </si>
   <si>
     <t>Figure comment</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Registration No.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Affiliation</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Figure file Name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Program No.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Program No. Long</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="6"/>
   </si>
   <si>
     <t>Acknowledgement</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="6"/>
   </si>
   <si>
     <t>Funding</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>References</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Session</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -86,14 +95,43 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="7">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Lucida Grande"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="2"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
+      <name val="Lucida Grande"/>
     </font>
     <font>
       <sz val="6"/>
@@ -101,29 +139,6 @@
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="2"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="11"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="2"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Lucida Grande"/>
     </font>
   </fonts>
   <fills count="2">
@@ -134,7 +149,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -142,43 +157,587 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="128">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="128">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="ハイパーリンク" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="標準" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="127" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -515,36 +1074,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E31" sqref="E31"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="25.625" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.375" style="1" customWidth="1"/>
-    <col min="2" max="3" width="14" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5" style="1" customWidth="1"/>
-    <col min="6" max="8" width="17.375" style="1" customWidth="1"/>
-    <col min="9" max="12" width="36" style="1" customWidth="1"/>
-    <col min="13" max="14" width="17.375" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="12.125" style="2"/>
+    <col min="1" max="1" width="3.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28" style="2" customWidth="1"/>
+    <col min="6" max="6" width="33" style="2" customWidth="1"/>
+    <col min="7" max="7" width="33.375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="24.125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="15" style="2" customWidth="1"/>
+    <col min="10" max="10" width="23.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="57.875" style="2" customWidth="1"/>
+    <col min="12" max="14" width="28.625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="22" style="2" customWidth="1"/>
+    <col min="16" max="16" width="43.875" style="2" customWidth="1"/>
+    <col min="17" max="16384" width="25.625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
+    <row r="1" spans="1:16" ht="31.5" customHeight="1">
+      <c r="A1" s="3"/>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -553,37 +1117,65 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="P1" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="D1:O1"/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.37" right="0.39000000000000007" top="0.8" bottom="0.41000000000000009" header="0.51" footer="0.51"/>
+  <pageSetup paperSize="8" scale="44" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13" defaultRowHeight="13.5"/>
+  <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>